<commit_message>
new info to metrics list
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Documents\Uni Mannheim\Master\IE 692 - Advanced Process Mining\TeamProject\process_complexity\replication\Rep_ImpactProcessComplexity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2608AC98-504B-4487-ADBF-DBE7B917CD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E08411-97B0-4B4B-8D21-D9137144A748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{82BBF392-2AF1-4CF6-ACD2-B00E9044F6AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Number of Events</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Unclear if "trace_length" is the same as "Min, Avg, Max"</t>
-  </si>
-  <si>
-    <t>Unclear if  "Affinity" is the same as "Distance Average Affinity"</t>
   </si>
   <si>
     <t>Unclear if "variety" is the same as "Variation Number of Acyclic Paths..."</t>
@@ -210,6 +207,28 @@
       </rPr>
       <t xml:space="preserve"> are used in the final model but there is no way known on how to compute them</t>
     </r>
+  </si>
+  <si>
+    <t>03.04.24: 
+Measure cant be calculated with the provided tool, throws an exception
+Unclear if  "Affinity" is the same as "Distance Average Affinity"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.04.24: 
+Measure cant be calculated with the provided tool, throws an exception
+</t>
+  </si>
+  <si>
+    <t>03.04.24:
+How to calculate the enriched variant entropy? With what is the normal variant entropy enriched?</t>
+  </si>
+  <si>
+    <t>03.04.24:
+The authors state that this measure can be calculated out of the box by PM4PY. However, I only found the method "pm4py.get_rework_cases_per_activity(log)" and this method only returns a dict of reps per process step. How to turn this into a valid metric?</t>
+  </si>
+  <si>
+    <t>03.04.24:
+What is this measure and how can it be computed?</t>
   </si>
 </sst>
 </file>
@@ -622,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4FE6D0-53EB-40A7-B72D-5501FB5C96B2}">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +658,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -647,10 +666,10 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
         <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>41</v>
@@ -658,7 +677,7 @@
     </row>
     <row r="4" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>0</v>
@@ -701,7 +720,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -720,27 +739,30 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G11" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="120" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -761,7 +783,7 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -782,7 +804,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
@@ -791,7 +813,7 @@
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
@@ -800,14 +822,14 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" ht="75" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>15</v>
       </c>
@@ -815,29 +837,32 @@
       <c r="F20" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:7" ht="180" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
         <v>19</v>
       </c>
@@ -845,8 +870,11 @@
       <c r="F24" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
         <v>20</v>
       </c>
@@ -855,7 +883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="7"/>
       <c r="E26" s="6" t="s">
         <v>24</v>
@@ -864,14 +892,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
         <v>27</v>
@@ -880,25 +908,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:7" ht="75" x14ac:dyDescent="0.25">
       <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change metrics.xlsx after resolving issue #1
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Documents\Uni Mannheim\Master\IE 692 - Advanced Process Mining\TeamProject\process_complexity\replication\Rep_ImpactProcessComplexity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E08411-97B0-4B4B-8D21-D9137144A748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE75D37-393B-4956-920C-66266702C70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{82BBF392-2AF1-4CF6-ACD2-B00E9044F6AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Number of Events</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Normalized variant entropy</t>
-  </si>
-  <si>
-    <t>Enriched Entropy Enriched Sequence entropy</t>
   </si>
   <si>
     <t xml:space="preserve">Enriched Variant entropy </t>
@@ -209,16 +206,6 @@
     </r>
   </si>
   <si>
-    <t>03.04.24: 
-Measure cant be calculated with the provided tool, throws an exception
-Unclear if  "Affinity" is the same as "Distance Average Affinity"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03.04.24: 
-Measure cant be calculated with the provided tool, throws an exception
-</t>
-  </si>
-  <si>
     <t>03.04.24:
 How to calculate the enriched variant entropy? With what is the normal variant entropy enriched?</t>
   </si>
@@ -229,6 +216,9 @@
   <si>
     <t>03.04.24:
 What is this measure and how can it be computed?</t>
+  </si>
+  <si>
+    <t>Enriched  Sequence entropy</t>
   </si>
 </sst>
 </file>
@@ -641,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4FE6D0-53EB-40A7-B72D-5501FB5C96B2}">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,26 +648,26 @@
   <sheetData>
     <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>0</v>
@@ -704,11 +694,11 @@
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -716,11 +706,11 @@
         <v>4</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -735,34 +725,28 @@
         <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>32</v>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -770,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -779,19 +763,19 @@
         <v>10</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="6"/>
     </row>
@@ -809,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="6"/>
     </row>
@@ -824,115 +808,112 @@
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="5" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="4:7" ht="75" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="4:7" ht="180" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="7"/>
       <c r="E26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="4:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="D30" s="6"/>
-      <c r="E30" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F30" s="6"/>
-      <c r="G30" s="4" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="31" spans="4:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>